<commit_message>
fixed mean weight plot
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -429,7 +429,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>1.5384615384615381</v>
+        <v>1.4705882352941173</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>1.5384615384615384E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>0.80622577482985502</v>
+        <v>0.82462112512353225</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="B9">
         <f>SQRT(B2)*B6</f>
-        <v>0.1</v>
+        <v>0.20000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>0.8</v>
+        <v>0.80000000000000016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>